<commit_message>
CV update for Cambridge
</commit_message>
<xml_diff>
--- a/cv_data/cv_entries.xlsx
+++ b/cv_data/cv_entries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/090f7abe46c7f02e/GitHub/ccl_cv/cv_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cclan\OneDrive\GitHub\ccl_cv\cv_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{EAB4230A-ADB7-4916-A22B-ACB2F2745C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FADF515-1F68-4E04-BD37-D1D4BDE0651A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B4A8E6-AFD0-4FE4-8883-B194D53B884B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="36105" windowHeight="15435" xr2:uid="{1BC556AC-FD23-42AD-A032-D140D4FFE02B}"/>
+    <workbookView xWindow="0" yWindow="3120" windowWidth="36105" windowHeight="15435" xr2:uid="{1BC556AC-FD23-42AD-A032-D140D4FFE02B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="167">
   <si>
     <t>type</t>
   </si>
@@ -511,6 +511,21 @@
   </si>
   <si>
     <t>Jun 2021</t>
+  </si>
+  <si>
+    <t>Institute of Criminology, University of Cambridge</t>
+  </si>
+  <si>
+    <t>Associate</t>
+  </si>
+  <si>
+    <t>Department of Sociology, Harvard University</t>
+  </si>
+  <si>
+    <t>Apr 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">University Assistant Professor (Beginning Sep. 2022) </t>
   </si>
 </sst>
 </file>
@@ -897,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2160BC3-6F18-4DB0-8375-6EA2E4BCFED4}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2061,6 +2076,37 @@
       </c>
       <c r="B67" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>152</v>
+      </c>
+      <c r="B68" t="s">
+        <v>166</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E68" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69" t="s">
+        <v>163</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E69" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Victims & Offenders review
</commit_message>
<xml_diff>
--- a/cv_data/cv_entries.xlsx
+++ b/cv_data/cv_entries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cclan\OneDrive\GitHub\ccl_cv\cv_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A82272B-6AEE-43E2-9AC5-4314784434BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A30C7EE-84D2-4CBF-87C6-5C18CB2200C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{1BC556AC-FD23-42AD-A032-D140D4FFE02B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{1BC556AC-FD23-42AD-A032-D140D4FFE02B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="250">
   <si>
     <t>type</t>
   </si>
@@ -772,6 +772,9 @@
   </si>
   <si>
     <t>https://clanfear.github.io/UW_2025-04-17/slides.html</t>
+  </si>
+  <si>
+    <t>Victims &amp; Offenders</t>
   </si>
 </sst>
 </file>
@@ -1165,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2160BC3-6F18-4DB0-8375-6EA2E4BCFED4}">
-  <dimension ref="A1:H112"/>
+  <dimension ref="A1:H113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="H110" sqref="H110"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3027,6 +3030,14 @@
       </c>
       <c r="H112" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A113" t="s">
+        <v>69</v>
+      </c>
+      <c r="B113" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CV moved to quarto
</commit_message>
<xml_diff>
--- a/cv_data/cv_entries.xlsx
+++ b/cv_data/cv_entries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/090f7abe46c7f02e/GitHub/ccl_cv/cv_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cl948\OneDrive\GitHub\ccl_cv\cv_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{7A30C7EE-84D2-4CBF-87C6-5C18CB2200C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C06EEBA2-93ED-4497-8496-B6E9B3E987D7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AE213A-EAA4-40FF-8E5D-EFCC21609051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="1740" windowWidth="38385" windowHeight="20865" xr2:uid="{1BC556AC-FD23-42AD-A032-D140D4FFE02B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{1BC556AC-FD23-42AD-A032-D140D4FFE02B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="253">
   <si>
     <t>type</t>
   </si>
@@ -781,6 +781,9 @@
   </si>
   <si>
     <t>Department of Sociology, University of Washington</t>
+  </si>
+  <si>
+    <t>The Lancet</t>
   </si>
 </sst>
 </file>
@@ -1174,23 +1177,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2160BC3-6F18-4DB0-8375-6EA2E4BCFED4}">
-  <dimension ref="A1:H114"/>
+  <dimension ref="A1:H115"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E114" sqref="E114"/>
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="5"/>
-    <col min="5" max="5" width="42.5703125" customWidth="1"/>
-    <col min="6" max="6" width="43.28515625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="2" max="2" width="57.54296875" customWidth="1"/>
+    <col min="3" max="4" width="9.1796875" style="5"/>
+    <col min="5" max="5" width="42.54296875" customWidth="1"/>
+    <col min="6" max="6" width="43.26953125" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1216,7 +1219,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>43608</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -1253,7 +1256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -1273,7 +1276,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1293,7 +1296,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1333,7 +1336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>47</v>
       </c>
@@ -1356,7 +1359,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -1379,7 +1382,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1396,7 +1399,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1413,7 +1416,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1430,7 +1433,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1444,7 +1447,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1461,7 +1464,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -1478,7 +1481,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1492,7 +1495,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1506,7 +1509,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1540,7 +1543,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1557,7 +1560,7 @@
         <v>42690</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1574,7 +1577,7 @@
         <v>42460</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1591,7 +1594,7 @@
         <v>41963</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1608,7 +1611,7 @@
         <v>41661</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -1625,7 +1628,7 @@
         <v>42459</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -1645,7 +1648,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -1665,7 +1668,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -1685,7 +1688,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -1702,7 +1705,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1736,7 +1739,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -1753,7 +1756,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>50</v>
       </c>
@@ -1770,7 +1773,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -1787,7 +1790,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -1804,7 +1807,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -1821,7 +1824,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -1847,7 +1850,7 @@
       </c>
       <c r="E37" s="3"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>44</v>
       </c>
@@ -1861,7 +1864,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -1878,7 +1881,7 @@
         <v>43783</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>19</v>
       </c>
@@ -1898,7 +1901,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -1915,7 +1918,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>47</v>
       </c>
@@ -1929,7 +1932,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>19</v>
       </c>
@@ -1949,7 +1952,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>19</v>
       </c>
@@ -1969,7 +1972,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -1986,7 +1989,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2003,7 +2006,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2020,7 +2023,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>91</v>
       </c>
@@ -2060,7 +2063,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>24</v>
       </c>
@@ -2074,7 +2077,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>163</v>
       </c>
@@ -2091,7 +2094,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>8</v>
       </c>
@@ -2108,7 +2111,7 @@
         <v>43481</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>8</v>
       </c>
@@ -2125,7 +2128,7 @@
         <v>42603</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>8</v>
       </c>
@@ -2142,7 +2145,7 @@
         <v>42602</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>8</v>
       </c>
@@ -2159,7 +2162,7 @@
         <v>44151</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>102</v>
       </c>
@@ -2176,7 +2179,7 @@
         <v>43398</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>91</v>
       </c>
@@ -2196,7 +2199,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>8</v>
       </c>
@@ -2216,7 +2219,7 @@
         <v>43735</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>69</v>
       </c>
@@ -2224,7 +2227,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -2232,7 +2235,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -2240,7 +2243,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>35</v>
       </c>
@@ -2260,7 +2263,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>24</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>129</v>
       </c>
@@ -2294,7 +2297,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>129</v>
       </c>
@@ -2311,7 +2314,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>35</v>
       </c>
@@ -2331,7 +2334,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>69</v>
       </c>
@@ -2339,7 +2342,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>129</v>
       </c>
@@ -2356,7 +2359,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>176</v>
       </c>
@@ -2373,7 +2376,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>23</v>
       </c>
@@ -2387,7 +2390,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -2395,7 +2398,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>47</v>
       </c>
@@ -2418,7 +2421,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>47</v>
       </c>
@@ -2441,7 +2444,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>8</v>
       </c>
@@ -2458,7 +2461,7 @@
         <v>44826</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>8</v>
       </c>
@@ -2475,7 +2478,7 @@
         <v>44883</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>8</v>
       </c>
@@ -2492,7 +2495,7 @@
         <v>44826</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>69</v>
       </c>
@@ -2500,7 +2503,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>69</v>
       </c>
@@ -2508,7 +2511,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>35</v>
       </c>
@@ -2528,7 +2531,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>69</v>
       </c>
@@ -2536,7 +2539,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>35</v>
       </c>
@@ -2553,7 +2556,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>163</v>
       </c>
@@ -2570,7 +2573,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>163</v>
       </c>
@@ -2587,7 +2590,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>163</v>
       </c>
@@ -2604,7 +2607,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>163</v>
       </c>
@@ -2621,7 +2624,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>163</v>
       </c>
@@ -2638,7 +2641,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>44</v>
       </c>
@@ -2655,7 +2658,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>44</v>
       </c>
@@ -2672,7 +2675,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>176</v>
       </c>
@@ -2689,7 +2692,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>69</v>
       </c>
@@ -2697,7 +2700,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>69</v>
       </c>
@@ -2705,7 +2708,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>8</v>
       </c>
@@ -2725,7 +2728,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>8</v>
       </c>
@@ -2745,7 +2748,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>35</v>
       </c>
@@ -2765,7 +2768,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>35</v>
       </c>
@@ -2782,7 +2785,7 @@
         <v>45227</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>69</v>
       </c>
@@ -2790,7 +2793,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>69</v>
       </c>
@@ -2798,7 +2801,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>8</v>
       </c>
@@ -2818,7 +2821,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>8</v>
       </c>
@@ -2838,7 +2841,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>8</v>
       </c>
@@ -2858,7 +2861,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>8</v>
       </c>
@@ -2878,7 +2881,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>8</v>
       </c>
@@ -2898,7 +2901,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>163</v>
       </c>
@@ -2915,7 +2918,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>35</v>
       </c>
@@ -2932,7 +2935,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>69</v>
       </c>
@@ -2940,7 +2943,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>8</v>
       </c>
@@ -2960,7 +2963,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>8</v>
       </c>
@@ -2980,7 +2983,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>69</v>
       </c>
@@ -2988,7 +2991,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>69</v>
       </c>
@@ -2996,7 +2999,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>69</v>
       </c>
@@ -3004,7 +3007,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>44</v>
       </c>
@@ -3018,7 +3021,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>8</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>69</v>
       </c>
@@ -3046,7 +3049,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>176</v>
       </c>
@@ -3055,6 +3058,14 @@
       </c>
       <c r="E114" t="s">
         <v>251</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A115" t="s">
+        <v>69</v>
+      </c>
+      <c r="B115" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>